<commit_message>
Finished world gen, fixed lack of tool restrictions, slight rearrangement of lines for better creative tab placement, moved to building materials tab
</commit_message>
<xml_diff>
--- a/Implementation Docs/Ore Gen.xlsx
+++ b/Implementation Docs/Ore Gen.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <t>Ore</t>
   </si>
@@ -45,22 +45,82 @@
     <t>Overworld Redstone</t>
   </si>
   <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Min Height</t>
   </si>
   <si>
     <t>Max Height</t>
+  </si>
+  <si>
+    <t>Nether Coal</t>
+  </si>
+  <si>
+    <t>Nether Diamond</t>
+  </si>
+  <si>
+    <t>Nether Emerald</t>
+  </si>
+  <si>
+    <t>Nether Gold</t>
+  </si>
+  <si>
+    <t>Nether Iron</t>
+  </si>
+  <si>
+    <t>Nether Lapis</t>
+  </si>
+  <si>
+    <t>Nether Redstone</t>
+  </si>
+  <si>
+    <t>Chances</t>
+  </si>
+  <si>
+    <t>Vein Size</t>
+  </si>
+  <si>
+    <t>Coded</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>getActualHeight()</t>
+  </si>
+  <si>
+    <t>End Coal</t>
+  </si>
+  <si>
+    <t>End Diamond</t>
+  </si>
+  <si>
+    <t>End Emerald</t>
+  </si>
+  <si>
+    <t>End Gold</t>
+  </si>
+  <si>
+    <t>End Iron</t>
+  </si>
+  <si>
+    <t>End Lapis</t>
+  </si>
+  <si>
+    <t>End Redstone</t>
+  </si>
+  <si>
+    <t>World-Gen</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Mining Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,17 +170,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8"/>
-  <sortState ref="A2:A8">
-    <sortCondition ref="A1:A8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22"/>
+  <sortState ref="A2:F22">
+    <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="8">
     <tableColumn id="1" name="Ore"/>
-    <tableColumn id="2" name="Size"/>
-    <tableColumn id="3" name="Count"/>
+    <tableColumn id="2" name="Vein Size"/>
+    <tableColumn id="3" name="Chances"/>
     <tableColumn id="4" name="Min Height"/>
     <tableColumn id="5" name="Max Height"/>
+    <tableColumn id="8" name="Mining Level"/>
+    <tableColumn id="6" name="Coded"/>
+    <tableColumn id="7" name="World-Gen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,148 +452,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
         <v>17</v>
       </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B19">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B20">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B21">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C21">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B22">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C22">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>16</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>